<commit_message>
update to use new id + description format
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data-template.xlsx
+++ b/tests/testthat/testdata/data-template.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -8,26 +8,1137 @@
   <sheets>
     <sheet name="Site data" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Site status" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Feature data" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Expectation of “z”" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Expectation of “x”" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Expectation of “c”" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Expectation of “v”" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Expectation of “b”" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Site feasibility" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Feature data" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Expectation of “z”" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Expectation of “x”" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Expectation of “c”" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Expectation of “v”" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Expectation of “b”" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>X</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action z</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action x</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action c</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action v</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action b</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site q</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site w</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site e</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site r</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site t</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>X</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action z</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action x</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action c</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action v</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action b</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site q</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site w</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site e</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site r</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site t</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>X</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action z</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action x</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action c</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action v</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Action b</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site q</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site w</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site e</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site r</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site t</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>X</author>
+  </authors>
+  <commentList>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature a</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature s</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature d</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature f</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature g</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>X</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature a</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature s</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature d</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature f</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature g</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site q</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site w</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site e</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site r</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site t</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>X</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature a</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature s</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature d</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature f</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature g</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site q</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site w</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site e</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site r</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site t</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>X</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature a</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature s</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature d</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature f</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature g</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site q</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site w</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site e</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site r</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site t</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>X</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature a</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature s</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature d</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature f</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature g</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site q</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site w</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site e</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site r</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site t</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>X</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature a</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature s</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature d</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature f</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature g</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site q</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site w</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site e</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site r</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Site t</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">Please enter information for your sites into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input the longitude and latitude (in decimal degrees) of each site. If you have a shapefile with spatial locations (e.g. point localities, boundaries) of your sites, these can also be supplied in the NCC Priority Actions App. We also ask that you input the cost of implementing each management action (e.g. in Canadian Dollars) within each site. Please note that cost values should not be below zero (though they can equal zero) and not be greater than 1,000,000 (i.e. one million). As such, you might need to rescale your cost values. For example, if one of your cost values is “10000000” Canadian Dollars, instead of inputting values as Canadian Dollars, you could you input values as thousands of Canadian Dollars (i.e. “10000”). Please take care to ensure that all cost values are in the same units. After filling out this worksheet, every light grey cell should have a numerical value.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Site name</t>
+    <t xml:space="preserve">Specifically, we ask that you input the longitude and latitude (in decimal degrees) of each site. If you have a shapefile with spatial locations (e.g. point localities, boundaries) of your sites, these can also be supplied in the NCC Priority Actions App. We also ask that you input the cost of implementing each management action (e.g. in Canadian Dollars) within each site. Please note that cost values should not be below zero (though they can equal zero) and not be greater than 1,000,000 (i.e. one million). As such, you might need to rescale your cost values. For example, if one of your cost values is “10000000” Canadian Dollars, instead of inputting values as Canadian Dollars, you could you input values as thousands of Canadian Dollars (i.e. “10000”). Please take care to ensure that all cost values are in the same units. After filling out this worksheet, every light gray cell should have a numerical value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site id</t>
   </si>
   <si>
     <t xml:space="preserve">Longitude (DD)</t>
@@ -72,7 +1183,7 @@
     <t xml:space="preserve">Please enter status information for your sites into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input data indicating which management actions can be implemented within each site. By default, all actions can be potentially implemented within each and every site. To specify that a certain a certain action cannot be implemented within a certain site, please enter value of “0”. You can also ensure that a certain site can ONLY have a certain action implemented within it, by specifying a value of “0” for every other action. This information, if you prefer, can also be specified within the NCC Priority Actions App---however, you will have to re-specify this information each and every time you open the NCC Priority Actions App.</t>
+    <t xml:space="preserve">Specifically, we ask that you input data indicating which management actions are currently being implemented within each site. By default, none of the actions are currently implemented within each site. To specify that a certain a certain action can be implemented within a certain site, please enter value of “1”. This information, if you prefer, can also be specified within the NCC Priority Actions App---however, you will have to re-specify this information each and every time you open the NCC Priority Actions App.</t>
   </si>
   <si>
     <t xml:space="preserve">Status of “z”</t>
@@ -90,13 +1201,34 @@
     <t xml:space="preserve">Status of “b”</t>
   </si>
   <si>
+    <t xml:space="preserve">Please enter feasibility information for your sites into this worksheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifically, we ask that you input data indicating which management actions are feasible to implement within each site. By default, all actions can be potentially implemented within each and every site. To specify that a certain a certain action cannot be implemented within a certain site, please enter value of “0”. You can also ensure that a certain site can ONLY have a certain action implemented within it, by specifying a value of “0” for every other action. This information, if you prefer, can also be specified within the NCC Priority Actions App---however, you will have to re-specify this information each and every time you open the NCC Priority Actions App.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feasibility of “z”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feasibility of “x”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feasibility of “c”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feasibility of “v”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feasibility of “b”</t>
+  </si>
+  <si>
     <t xml:space="preserve">Please enter information for your features into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input values to specify trade-offs for managing different biodiversity elements (e.g. species, habitat types) within your conservation planning exercise. To help prioritise implementation of specific management actions in specific sites, we require an estimate of the minimum amount of each feature you think is important to achieve across all of the sites (termed “target threshold amount”). For example, you could calculate these target threshold amounts as a percentage of the current amount of each feature (e.g. maybe you want to increase the amount of each feature by 50%)? Alternatively, these values could be guided using population viability analyses, statistical models, or expert elicitation. Please take care to ensure that each target value is in the same units as the expectation data. For example, the value in the cell B2 for this spreadsheet should be in the same unit as the values in the B column for all action expectation worksheets (i.e. worksheets starting with the word “Expectation”). To ensure that the prioritization process explicitly accounts for your objectives (i.e. what YOU think is important), you can also specify the relative importance (weight) of each feature. The default value is 1 such that all features are considered equally important. These values should be between 0 and 100. Greater values indicate greater importance. A weight of exactly 0 means that a feature is not important at all and does not “count” when comparing different conservation plans. Please note that these values can be changed later in the NCC Priority Actions App. After filling out this worksheet, every light grey cell should have a numerical value.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feature name</t>
+    <t xml:space="preserve">Specifically, we ask that you input values to specify trade-offs for managing different biodiversity elements (e.g. species, habitat types) within your conservation planning exercise. To help prioritize implementation of specific management actions in specific sites, we require an estimate of the minimum amount of each feature you think is important to achieve across all of the sites (termed “target threshold amount”). For example, you could calculate these target threshold amounts as a percentage of the current amount of each feature (e.g. maybe you want to increase the amount of each feature by 50%)? Alternatively, these values could be guided using population viability analyses, statistical models, or expert elicitation. Please take care to ensure that each target value is in the same units as the expectation data. For example, the value in the cell B2 for this spreadsheet should be in the same unit as the values in the B column for all action expectation worksheets (i.e. worksheets starting with the word “Expectation”). To ensure that the prioritization process explicitly accounts for your objectives (i.e. what YOU think is important), you can also specify the relative importance (weight) of each feature. The default value is 1 such that all features are considered equally important. These values should be between 0 and 100. Greater values indicate greater importance. A weight of exactly 0 means that a feature is not important at all and does not “count” when comparing different conservation plans. Please note that these values can be changed later in the NCC Priority Actions App. After filling out this worksheet, every light gray cell should have a numerical value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature id</t>
   </si>
   <si>
     <t xml:space="preserve">Target threshold amount</t>
@@ -123,7 +1255,7 @@
     <t xml:space="preserve">Please enter information for your “z” action into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “z” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light grey cell should have a numerical value.</t>
+    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “z” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
   </si>
   <si>
     <t xml:space="preserve">Amount of “a”</t>
@@ -144,31 +1276,31 @@
     <t xml:space="preserve">Please enter information for your “x” action into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “x” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light grey cell should have a numerical value.</t>
+    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “x” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
   </si>
   <si>
     <t xml:space="preserve">Please enter information for your “c” action into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “c” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light grey cell should have a numerical value.</t>
+    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “c” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
   </si>
   <si>
     <t xml:space="preserve">Please enter information for your “v” action into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “v” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light grey cell should have a numerical value.</t>
+    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “v” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
   </si>
   <si>
     <t xml:space="preserve">Please enter information for your “b” action into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “b” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light grey cell should have a numerical value.</t>
+    <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “b” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="7">
     <font>
@@ -369,7 +1501,22 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Site name"/>
+    <tableColumn id="1" name="Site id"/>
+    <tableColumn id="2" name="Amount of “a”"/>
+    <tableColumn id="3" name="Amount of “s”"/>
+    <tableColumn id="4" name="Amount of “d”"/>
+    <tableColumn id="5" name="Amount of “f”"/>
+    <tableColumn id="6" name="Amount of “g”"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:F8"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Site id"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>
@@ -384,7 +1531,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:H8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:H8"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Site name"/>
+    <tableColumn id="1" name="Site id"/>
     <tableColumn id="2" name="Longitude (DD)"/>
     <tableColumn id="3" name="Latitude (DD)"/>
     <tableColumn id="4" name="Cost of “z”"/>
@@ -401,7 +1548,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Site name"/>
+    <tableColumn id="1" name="Site id"/>
     <tableColumn id="2" name="Status of “z”"/>
     <tableColumn id="3" name="Status of “x”"/>
     <tableColumn id="4" name="Status of “c”"/>
@@ -413,27 +1560,27 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A3:C8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:C8"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Feature name"/>
-    <tableColumn id="2" name="Target threshold amount"/>
-    <tableColumn id="3" name="Relative importance (weight)"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:F8"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Site id"/>
+    <tableColumn id="2" name="Feasibility of “z”"/>
+    <tableColumn id="3" name="Feasibility of “x”"/>
+    <tableColumn id="4" name="Feasibility of “c”"/>
+    <tableColumn id="5" name="Feasibility of “v”"/>
+    <tableColumn id="6" name="Feasibility of “b”"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:F8"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Site name"/>
-    <tableColumn id="2" name="Amount of “a”"/>
-    <tableColumn id="3" name="Amount of “s”"/>
-    <tableColumn id="4" name="Amount of “d”"/>
-    <tableColumn id="5" name="Amount of “f”"/>
-    <tableColumn id="6" name="Amount of “g”"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A3:C8" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:C8"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Feature id"/>
+    <tableColumn id="2" name="Target threshold amount"/>
+    <tableColumn id="3" name="Relative importance (weight)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -443,7 +1590,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Site name"/>
+    <tableColumn id="1" name="Site id"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>
@@ -458,7 +1605,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Site name"/>
+    <tableColumn id="1" name="Site id"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>
@@ -473,7 +1620,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Site name"/>
+    <tableColumn id="1" name="Site id"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>
@@ -762,16 +1909,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1">
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="19.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="24.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="21.71" hidden="0" customWidth="1"/>
@@ -933,6 +2080,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <legacyDrawing r:id="rIdvml"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
   </tableParts>
@@ -940,16 +2088,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0">
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="19.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="23.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
@@ -1002,19 +2150,19 @@
         <v>10</v>
       </c>
       <c r="B4" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1022,19 +2170,19 @@
         <v>12</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1042,19 +2190,19 @@
         <v>13</v>
       </c>
       <c r="B6" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1062,19 +2210,19 @@
         <v>14</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1082,19 +2230,19 @@
         <v>15</v>
       </c>
       <c r="B8" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1119,6 +2267,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <legacyDrawing r:id="rIdvml"/>
   <tableParts count="1">
     <tablePart r:id="rId4"/>
   </tableParts>
@@ -1126,16 +2275,203 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0">
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="22.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="28.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="28.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="28.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="28.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="28.71" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" ht="100" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B4:F8">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>B4=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>B4=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:F8">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <legacyDrawing r:id="rIdvml"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="20.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="33.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="38.71" hidden="0" customWidth="1"/>
   </cols>
@@ -1143,31 +2479,31 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" ht="250" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
@@ -1178,7 +2514,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>11</v>
@@ -1189,7 +2525,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
@@ -1200,7 +2536,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>11</v>
@@ -1211,7 +2547,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>11</v>
@@ -1238,23 +2574,24 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <legacyDrawing r:id="rIdvml"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0">
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="19.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="23.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
@@ -1265,7 +2602,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1275,7 +2612,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1287,19 +2624,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
@@ -1366,23 +2703,24 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <legacyDrawing r:id="rIdvml"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0">
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="19.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="23.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
@@ -1393,7 +2731,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1403,7 +2741,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1415,19 +2753,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
@@ -1494,23 +2832,24 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <legacyDrawing r:id="rIdvml"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0">
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="19.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="23.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
@@ -1521,7 +2860,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1531,7 +2870,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1543,19 +2882,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
@@ -1622,23 +2961,24 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <legacyDrawing r:id="rIdvml"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0">
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="19.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="23.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
@@ -1649,7 +2989,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1659,7 +2999,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1671,19 +3011,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
@@ -1750,23 +3090,24 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <legacyDrawing r:id="rIdvml"/>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0">
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="19.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="23.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
@@ -1777,7 +3118,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1787,7 +3128,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1799,19 +3140,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
@@ -1878,8 +3219,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <legacyDrawing r:id="rIdvml"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update colors in template styles
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data-template.xlsx
+++ b/tests/testthat/testdata/data-template.xlsx
@@ -1138,7 +1138,7 @@
     <t xml:space="preserve">Specifically, we ask that you input the longitude and latitude (in decimal degrees) of each site. If you have a shapefile with spatial locations (e.g. point localities, boundaries) of your sites, these can also be supplied in the NCC Priority Actions App. We also ask that you input the cost of implementing each management action (e.g. in Canadian Dollars) within each site. Please note that cost values should not be below zero (though they can equal zero) and not be greater than 1,000,000 (i.e. one million). As such, you might need to rescale your cost values. For example, if one of your cost values is “10000000” Canadian Dollars, instead of inputting values as Canadian Dollars, you could you input values as thousands of Canadian Dollars (i.e. “10000”). Please take care to ensure that all cost values are in the same units. After filling out this worksheet, every light gray cell should have a numerical value.</t>
   </si>
   <si>
-    <t xml:space="preserve">Site id</t>
+    <t xml:space="preserve">Site ID</t>
   </si>
   <si>
     <t xml:space="preserve">Longitude (DD)</t>
@@ -1228,7 +1228,7 @@
     <t xml:space="preserve">Specifically, we ask that you input values to specify trade-offs for managing different biodiversity elements (e.g. species, habitat types) within your conservation planning exercise. To help prioritize implementation of specific management actions in specific sites, we require an estimate of the minimum amount of each feature you think is important to achieve across all of the sites (termed “target threshold amount”). For example, you could calculate these target threshold amounts as a percentage of the current amount of each feature (e.g. maybe you want to increase the amount of each feature by 50%)? Alternatively, these values could be guided using population viability analyses, statistical models, or expert elicitation. Please take care to ensure that each target value is in the same units as the expectation data. For example, the value in the cell B2 for this spreadsheet should be in the same unit as the values in the B column for all action expectation worksheets (i.e. worksheets starting with the word “Expectation”). To ensure that the prioritization process explicitly accounts for your objectives (i.e. what YOU think is important), you can also specify the relative importance (weight) of each feature. The default value is 1 such that all features are considered equally important. These values should be between 0 and 100. Greater values indicate greater importance. A weight of exactly 0 means that a feature is not important at all and does not “count” when comparing different conservation plans. Please note that these values can be changed later in the NCC Priority Actions App. After filling out this worksheet, every light gray cell should have a numerical value.</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature id</t>
+    <t xml:space="preserve">Feature ID</t>
   </si>
   <si>
     <t xml:space="preserve">Target threshold amount</t>
@@ -1323,18 +1323,18 @@
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FF000063"/>
+      <color rgb="FF283B39"/>
       <name val="Times New Roman"/>
       <b/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000081"/>
+      <color rgb="FF283B39"/>
       <name val="Times New Roman"/>
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF283B39"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -1358,14 +1358,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCFCFCF"/>
-        <bgColor rgb="FFCFCFCF"/>
+        <fgColor rgb="FF7B9D7A"/>
+        <bgColor rgb="FF7B9D7A"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE3E3E3"/>
-        <bgColor rgb="FFE3E3E3"/>
+        <fgColor rgb="FFE3DCD7"/>
+        <bgColor rgb="FFE3DCD7"/>
       </patternFill>
     </fill>
   </fills>
@@ -1393,16 +1393,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF283B39"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF283B39"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF283B39"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF283B39"/>
       </bottom>
     </border>
   </borders>
@@ -1419,11 +1419,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="1"/>
     </xf>
@@ -1442,13 +1442,13 @@
     <dxf>
       <font>
         <sz val="12"/>
-        <color rgb="FFC10100"/>
+        <color rgb="FFB12F31"/>
         <name val="Arial"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFF87D18"/>
-          <bgColor rgb="FFF87D18"/>
+          <fgColor rgb="FFF96E67"/>
+          <bgColor rgb="FFF96E67"/>
         </patternFill>
       </fill>
       <border>
@@ -1469,13 +1469,13 @@
     <dxf>
       <font>
         <sz val="12"/>
-        <color rgb="FF5A7C00"/>
+        <color rgb="FF115D2F"/>
         <name val="Arial"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF9FAA13"/>
-          <bgColor rgb="FF9FAA13"/>
+          <fgColor rgb="FF4CBC89"/>
+          <bgColor rgb="FF4CBC89"/>
         </patternFill>
       </fill>
       <border>
@@ -1501,7 +1501,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Site id"/>
+    <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>
@@ -1516,7 +1516,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Site id"/>
+    <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>
@@ -1531,7 +1531,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:H8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:H8"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Site id"/>
+    <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Longitude (DD)"/>
     <tableColumn id="3" name="Latitude (DD)"/>
     <tableColumn id="4" name="Cost of “z”"/>
@@ -1548,7 +1548,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Site id"/>
+    <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Status of “z”"/>
     <tableColumn id="3" name="Status of “x”"/>
     <tableColumn id="4" name="Status of “c”"/>
@@ -1563,7 +1563,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Site id"/>
+    <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Feasibility of “z”"/>
     <tableColumn id="3" name="Feasibility of “x”"/>
     <tableColumn id="4" name="Feasibility of “c”"/>
@@ -1578,7 +1578,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A3:C8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:C8"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Feature id"/>
+    <tableColumn id="1" name="Feature ID"/>
     <tableColumn id="2" name="Target threshold amount"/>
     <tableColumn id="3" name="Relative importance (weight)"/>
   </tableColumns>
@@ -1590,7 +1590,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Site id"/>
+    <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>
@@ -1605,7 +1605,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Site id"/>
+    <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>
@@ -1620,7 +1620,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Site id"/>
+    <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>

</xml_diff>

<commit_message>
refactor status and feasibility sheet data
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data-template.xlsx
+++ b/tests/testthat/testdata/data-template.xlsx
@@ -7,8 +7,8 @@
   </bookViews>
   <sheets>
     <sheet name="Site data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Site status" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Site feasibility" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Status data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Feasibility data" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Feature data" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Expectation of “z”" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Expectation of “x”" sheetId="6" state="visible" r:id="rId6"/>
@@ -155,6 +155,18 @@
     <author>X</author>
   </authors>
   <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">...1</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <r>
@@ -285,6 +297,18 @@
     <author>X</author>
   </authors>
   <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">...1</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <r>

</xml_diff>

<commit_message>
current status is now a column
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data-template.xlsx
+++ b/tests/testthat/testdata/data-template.xlsx
@@ -7,14 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Site data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Status data" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Feasibility data" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Feature data" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Expectation of “z”" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Expectation of “x”" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Expectation of “c”" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Expectation of “v”" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Expectation of “b”" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Feasibility data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Feature data" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Expectation of “z”" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Expectation of “x”" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Expectation of “c”" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Expectation of “v”" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Expectation of “b”" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -25,7 +24,7 @@
     <author>X</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -37,7 +36,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
+    <comment ref="G3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0" shapeId="0">
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0">
+    <comment ref="I3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -155,18 +154,6 @@
     <author>X</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">...1</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <r>
@@ -297,78 +284,6 @@
     <author>X</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">...1</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Action z</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Action x</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Action c</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Action v</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Action b</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -377,7 +292,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Site q</t>
+          <t xml:space="preserve">Feature a</t>
         </r>
       </text>
     </comment>
@@ -389,7 +304,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Site w</t>
+          <t xml:space="preserve">Feature s</t>
         </r>
       </text>
     </comment>
@@ -401,7 +316,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Site e</t>
+          <t xml:space="preserve">Feature d</t>
         </r>
       </text>
     </comment>
@@ -413,7 +328,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Site r</t>
+          <t xml:space="preserve">Feature f</t>
         </r>
       </text>
     </comment>
@@ -425,7 +340,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Site t</t>
+          <t xml:space="preserve">Feature g</t>
         </r>
       </text>
     </comment>
@@ -439,6 +354,66 @@
     <author>X</author>
   </authors>
   <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature a</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature s</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature d</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature f</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <name val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Feature g</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -447,7 +422,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Feature a</t>
+          <t xml:space="preserve">Site q</t>
         </r>
       </text>
     </comment>
@@ -459,7 +434,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Feature s</t>
+          <t xml:space="preserve">Site w</t>
         </r>
       </text>
     </comment>
@@ -471,7 +446,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Feature d</t>
+          <t xml:space="preserve">Site e</t>
         </r>
       </text>
     </comment>
@@ -483,7 +458,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Feature f</t>
+          <t xml:space="preserve">Site r</t>
         </r>
       </text>
     </comment>
@@ -495,7 +470,7 @@
             <color rgb="FF000000"/>
             <name val="Tahoma"/>
           </rPr>
-          <t xml:space="preserve">Feature g</t>
+          <t xml:space="preserve">Site t</t>
         </r>
       </text>
     </comment>
@@ -1023,138 +998,8 @@
 </comments>
 </file>
 
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>X</author>
-  </authors>
-  <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Feature a</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Feature s</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Feature d</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Feature f</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Feature g</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site q</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site w</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site e</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site r</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site t</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t xml:space="preserve">Please enter information for your sites into this worksheet.</t>
   </si>
@@ -1171,6 +1016,9 @@
     <t xml:space="preserve">Latitude (DD)</t>
   </si>
   <si>
+    <t xml:space="preserve">Current status</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cost of “z”</t>
   </si>
   <si>
@@ -1202,27 +1050,6 @@
   </si>
   <si>
     <t xml:space="preserve">t</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please enter status information for your sites into this worksheet.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specifically, we ask that you input data indicating which management actions are currently being implemented within each site. By default, none of the actions are currently implemented within each site. To specify that a certain a certain action can be implemented within a certain site, please enter value of “1”. This information, if you prefer, can also be specified within the NCC Priority Actions App---however, you will have to re-specify this information each and every time you open the NCC Priority Actions App.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status of “z”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status of “x”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status of “c”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status of “v”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status of “b”</t>
   </si>
   <si>
     <t xml:space="preserve">Please enter feasibility information for your sites into this worksheet.</t>
@@ -1536,33 +1363,19 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:F8"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Site ID"/>
-    <tableColumn id="2" name="Amount of “a”"/>
-    <tableColumn id="3" name="Amount of “s”"/>
-    <tableColumn id="4" name="Amount of “d”"/>
-    <tableColumn id="5" name="Amount of “f”"/>
-    <tableColumn id="6" name="Amount of “g”"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:H8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:H8"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:I8" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:I8"/>
+  <tableColumns count="9">
     <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Longitude (DD)"/>
     <tableColumn id="3" name="Latitude (DD)"/>
-    <tableColumn id="4" name="Cost of “z”"/>
-    <tableColumn id="5" name="Cost of “x”"/>
-    <tableColumn id="6" name="Cost of “c”"/>
-    <tableColumn id="7" name="Cost of “v”"/>
-    <tableColumn id="8" name="Cost of “b”"/>
+    <tableColumn id="4" name="Current status"/>
+    <tableColumn id="5" name="Cost of “z”"/>
+    <tableColumn id="6" name="Cost of “x”"/>
+    <tableColumn id="7" name="Cost of “c”"/>
+    <tableColumn id="8" name="Cost of “v”"/>
+    <tableColumn id="9" name="Cost of “b”"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1570,21 +1383,6 @@
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:F8"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Site ID"/>
-    <tableColumn id="2" name="Status of “z”"/>
-    <tableColumn id="3" name="Status of “x”"/>
-    <tableColumn id="4" name="Status of “c”"/>
-    <tableColumn id="5" name="Status of “v”"/>
-    <tableColumn id="6" name="Status of “b”"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:F8"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Site ID"/>
@@ -1598,13 +1396,28 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A3:C8" totalsRowCount="0" totalsRowShown="0">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A3:C8" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A3:C8"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Feature ID"/>
     <tableColumn id="2" name="Target threshold amount"/>
     <tableColumn id="3" name="Relative importance (weight)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:F8"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Site ID"/>
+    <tableColumn id="2" name="Amount of “a”"/>
+    <tableColumn id="3" name="Amount of “s”"/>
+    <tableColumn id="4" name="Amount of “d”"/>
+    <tableColumn id="5" name="Amount of “f”"/>
+    <tableColumn id="6" name="Amount of “g”"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1945,11 +1758,12 @@
     <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="24.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="21.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="24.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="21.71" hidden="0" customWidth="1"/>
     <col min="6" max="6" width="21.71" hidden="0" customWidth="1"/>
     <col min="7" max="7" width="21.71" hidden="0" customWidth="1"/>
     <col min="8" max="8" width="21.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="21.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1963,6 +1777,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" ht="120" customHeight="1">
       <c r="A2" s="2"/>
@@ -1975,6 +1790,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
@@ -2001,86 +1817,104 @@
       <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="I3" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
@@ -2097,7 +1931,7 @@
       <formula1>-90</formula1>
       <formula2>90</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="D4:H8">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="E4:I8">
       <formula1>0</formula1>
       <formula2>1e+06</formula2>
     </dataValidation>
@@ -2108,6 +1942,18 @@
   <tableParts count="1">
     <tablePart r:id="rId3"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Site data'!$A$4:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>D4:D8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2122,17 +1968,17 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="23.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="23.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="23.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="28.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="28.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="28.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="28.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="28.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2142,7 +1988,7 @@
     <row r="2" ht="100" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2154,119 +2000,119 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2308,152 +2154,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="28.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="28.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="28.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="28.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="28.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="20.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="33.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="38.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" ht="100" customHeight="1">
+    </row>
+    <row r="2" ht="250" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="6" t="n">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>1</v>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="6" t="n">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2462,18 +2245,14 @@
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F8">
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>B4=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>B4=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="whole" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:F8">
+  <dataValidations count="2">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:B8">
       <formula1>0</formula1>
-      <formula2>1</formula2>
+      <formula2>1e+06</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="C4:C8">
+      <formula1>0</formula1>
+      <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2495,90 +2274,103 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="20.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="33.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="38.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="23.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="23.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="23.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1"/>
-    </row>
-    <row r="2" ht="250" customHeight="1">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
@@ -2586,14 +2378,10 @@
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:B8">
+  <dataValidations count="1">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:F8">
       <formula1>0</formula1>
-      <formula2>1e+06</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="C4:C8">
-      <formula1>0</formula1>
-      <formula2>100</formula2>
+      <formula2>10000</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2626,7 +2414,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2636,7 +2424,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2648,24 +2436,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2675,7 +2463,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2685,7 +2473,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2695,7 +2483,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2705,7 +2493,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2755,7 +2543,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2765,7 +2553,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2777,24 +2565,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2804,7 +2592,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2814,7 +2602,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2824,7 +2612,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2834,7 +2622,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2884,7 +2672,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2894,7 +2682,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2906,24 +2694,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2933,7 +2721,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2943,7 +2731,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2953,7 +2741,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2963,7 +2751,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -3013,7 +2801,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -3023,7 +2811,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -3035,24 +2823,24 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -3062,7 +2850,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -3072,7 +2860,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3082,7 +2870,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -3092,7 +2880,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -3119,133 +2907,4 @@
     <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <cols>
-    <col min="1" max="1" width="17.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="23.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
-    <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
-    <col min="5" max="5" width="23.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="23.71" hidden="0" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="20" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" ht="160" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
-  <mergeCells count="2">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:F8">
-      <formula1>0</formula1>
-      <formula2>10000</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-  <legacyDrawing r:id="rIdvml"/>
-  <tableParts count="1">
-    <tablePart r:id="rId11"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add validation for current status
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data-template.xlsx
+++ b/tests/testthat/testdata/data-template.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Expectation of “c”" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Expectation of “v”" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Expectation of “b”" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="meta" sheetId="9" state="hidden" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
@@ -999,7 +1000,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t xml:space="preserve">Please enter information for your sites into this worksheet.</t>
   </si>
@@ -1146,6 +1147,30 @@
   </si>
   <si>
     <t xml:space="preserve">Specifically, we ask that you input the amount of each biodiversity element (termed feature) that you would expect to occur within each site after you implemented the “b” action. For example, these values could indicate that you expect a certain feature (e.g. species) to be present (using a value of “1”) or absent (using a value of “0”) within certain sites after this action is implemented. Alternatively, these could represent quantities such as expected population size (using count values) or amount of habitat (in km^2). Although different feature can have different units, each feature must have values in the same units. Thus all rows in the same column within this worksheet must be in the same units. Additionally, across worksheets for different actions (i.e. those starting with the word “Expectation”), the values in the same column must be in the same units (e.g. all values in the column B in each of these of these action worksheets must have the same units). After filling out this worksheet, every light gray cell should have a numerical value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site_ids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action_ids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feature_ids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
   </si>
 </sst>
 </file>
@@ -1358,6 +1383,18 @@
     <tableColumn id="4" name="Amount of “d”"/>
     <tableColumn id="5" name="Amount of “f”"/>
     <tableColumn id="6" name="Amount of “g”"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:C6" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:C6"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="site_ids"/>
+    <tableColumn id="2" name="action_ids"/>
+    <tableColumn id="3" name="feature_ids"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1947,7 +1984,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'Site data'!$A$4:$A$8</xm:f>
+            <xm:f>'meta'!$B$2:$B$6</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D8</xm:sqref>
         </x14:dataValidation>
@@ -2907,4 +2944,88 @@
     <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId11"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
store descriptions in meta sheet
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data-template.xlsx
+++ b/tests/testthat/testdata/data-template.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Expectation of “c”" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Expectation of “v”" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Expectation of “b”" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="meta" sheetId="9" state="hidden" r:id="rId9"/>
+    <sheet name="metadata" sheetId="9" state="hidden" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
@@ -121,30 +121,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site r</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site t</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -251,30 +227,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site r</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site t</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -333,18 +285,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Feature g</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -403,18 +343,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Feature g</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -448,30 +376,6 @@
             <name val="Tahoma"/>
           </rPr>
           <t xml:space="preserve">Site e</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site r</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site t</t>
         </r>
       </text>
     </comment>
@@ -533,18 +437,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Feature g</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -578,30 +470,6 @@
             <name val="Tahoma"/>
           </rPr>
           <t xml:space="preserve">Site e</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site r</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site t</t>
         </r>
       </text>
     </comment>
@@ -663,18 +531,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Feature g</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -708,30 +564,6 @@
             <name val="Tahoma"/>
           </rPr>
           <t xml:space="preserve">Site e</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site r</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site t</t>
         </r>
       </text>
     </comment>
@@ -793,18 +625,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Feature g</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -838,30 +658,6 @@
             <name val="Tahoma"/>
           </rPr>
           <t xml:space="preserve">Site e</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site r</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site t</t>
         </r>
       </text>
     </comment>
@@ -923,18 +719,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Feature g</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
@@ -968,30 +752,6 @@
             <name val="Tahoma"/>
           </rPr>
           <t xml:space="preserve">Site e</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site r</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <name val="Tahoma"/>
-          </rPr>
-          <t xml:space="preserve">Site t</t>
         </r>
       </text>
     </comment>
@@ -1000,7 +760,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t xml:space="preserve">Please enter information for your sites into this worksheet.</t>
   </si>
@@ -1047,12 +807,6 @@
     <t xml:space="preserve">e</t>
   </si>
   <si>
-    <t xml:space="preserve">r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please enter feasibility information for your sites into this worksheet.</t>
   </si>
   <si>
@@ -1101,9 +855,6 @@
     <t xml:space="preserve">f</t>
   </si>
   <si>
-    <t xml:space="preserve">g</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please enter information for your “z” action into this worksheet.</t>
   </si>
   <si>
@@ -1122,9 +873,6 @@
     <t xml:space="preserve">Amount of “f”</t>
   </si>
   <si>
-    <t xml:space="preserve">Amount of “g”</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please enter information for your “x” action into this worksheet.</t>
   </si>
   <si>
@@ -1158,19 +906,64 @@
     <t xml:space="preserve">feature_ids</t>
   </si>
   <si>
+    <t xml:space="preserve">site_descriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action_descriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feature_descriptions</t>
+  </si>
+  <si>
     <t xml:space="preserve">z</t>
   </si>
   <si>
+    <t xml:space="preserve">Site q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature a</t>
+  </si>
+  <si>
     <t xml:space="preserve">x</t>
   </si>
   <si>
+    <t xml:space="preserve">Site w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature s</t>
+  </si>
+  <si>
     <t xml:space="preserve">c</t>
   </si>
   <si>
+    <t xml:space="preserve">Site e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature d</t>
+  </si>
+  <si>
     <t xml:space="preserve">v</t>
   </si>
   <si>
+    <t xml:space="preserve">Action v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature f</t>
+  </si>
+  <si>
     <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action b</t>
   </si>
 </sst>
 </file>
@@ -1374,35 +1167,37 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:F8"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A3:E6" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:E6"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>
     <tableColumn id="5" name="Amount of “f”"/>
-    <tableColumn id="6" name="Amount of “g”"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:C6" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:C6"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:F6" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:F6"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="site_ids"/>
     <tableColumn id="2" name="action_ids"/>
     <tableColumn id="3" name="feature_ids"/>
+    <tableColumn id="4" name="site_descriptions"/>
+    <tableColumn id="5" name="action_descriptions"/>
+    <tableColumn id="6" name="feature_descriptions"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:I8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:I8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A3:I6" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:I6"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Longitude (DD)"/>
@@ -1419,8 +1214,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:F8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A3:F6" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:F6"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Feasibility of “z”"/>
@@ -1434,8 +1229,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A3:C8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:C8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A3:C7" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:C7"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Feature ID"/>
     <tableColumn id="2" name="Target threshold amount"/>
@@ -1446,60 +1241,56 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:F8"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A3:E6" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:E6"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>
     <tableColumn id="5" name="Amount of “f”"/>
-    <tableColumn id="6" name="Amount of “g”"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:F8"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A3:E6" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:E6"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>
     <tableColumn id="5" name="Amount of “f”"/>
-    <tableColumn id="6" name="Amount of “g”"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:F8"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A3:E6" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:E6"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>
     <tableColumn id="5" name="Amount of “f”"/>
-    <tableColumn id="6" name="Amount of “g”"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A3:F8" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A3:F8"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A3:E6" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A3:E6"/>
+  <tableColumns count="5">
     <tableColumn id="1" name="Site ID"/>
     <tableColumn id="2" name="Amount of “a”"/>
     <tableColumn id="3" name="Amount of “s”"/>
     <tableColumn id="4" name="Amount of “d”"/>
     <tableColumn id="5" name="Amount of “f”"/>
-    <tableColumn id="6" name="Amount of “g”"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1915,44 +1706,6 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
   <mergeCells count="2">
@@ -1960,15 +1713,15 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:B8">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:B6">
       <formula1>-180</formula1>
       <formula2>180</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="C4:C8">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="C4:C6">
       <formula1>-90</formula1>
       <formula2>90</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="E4:I8">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="E4:I6">
       <formula1>0</formula1>
       <formula2>1e+06</formula2>
     </dataValidation>
@@ -1986,7 +1739,7 @@
           <x14:formula1>
             <xm:f>'meta'!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D4:D8</xm:sqref>
+          <xm:sqref>D4:D6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2015,7 +1768,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2025,7 +1778,7 @@
     <row r="2" ht="100" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2037,19 +1790,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -2109,46 +1862,6 @@
         <v>1</v>
       </c>
       <c r="F6" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2158,7 +1871,7 @@
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F8">
+  <conditionalFormatting sqref="B4:F6">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>B4=0</formula>
     </cfRule>
@@ -2167,7 +1880,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:F8">
+    <dataValidation type="whole" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:F6">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -2199,31 +1912,31 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" ht="250" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>12</v>
@@ -2234,7 +1947,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>12</v>
@@ -2245,7 +1958,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>12</v>
@@ -2256,23 +1969,12 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2283,11 +1985,11 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:B8">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:B7">
       <formula1>0</formula1>
       <formula2>1e+06</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="C4:C8">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="C4:C7">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2316,47 +2018,41 @@
     <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="23.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="23.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
     </row>
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -2367,7 +2063,6 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
@@ -2377,7 +2072,6 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
@@ -2387,27 +2081,6 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
@@ -2416,7 +2089,7 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:F8">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:E6">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2445,47 +2118,41 @@
     <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="23.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="23.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
     </row>
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -2496,7 +2163,6 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
@@ -2506,7 +2172,6 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
@@ -2516,27 +2181,6 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
@@ -2545,7 +2189,7 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:F8">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:E6">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2574,47 +2218,41 @@
     <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="23.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="23.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
     </row>
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -2625,7 +2263,6 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
@@ -2635,7 +2272,6 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
@@ -2645,27 +2281,6 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
@@ -2674,7 +2289,7 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:F8">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:E6">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2703,47 +2318,41 @@
     <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="23.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="23.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
     </row>
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -2754,7 +2363,6 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
@@ -2764,7 +2372,6 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
@@ -2774,27 +2381,6 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
@@ -2803,7 +2389,7 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:F8">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:E6">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2832,47 +2418,41 @@
     <col min="3" max="3" width="23.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="23.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="23.71" hidden="0" customWidth="1"/>
-    <col min="6" max="6" width="23.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
     </row>
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4">
@@ -2883,7 +2463,6 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
@@ -2893,7 +2472,6 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
@@ -2903,27 +2481,6 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" insertColumns="1" insertRows="1" deleteColumns="1" deleteRows="1" sheet="1"/>
@@ -2932,7 +2489,7 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:F8">
+    <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:E6">
       <formula1>0</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -2956,13 +2513,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2">
@@ -2970,10 +2536,19 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" t="s">
-        <v>29</v>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3">
@@ -2981,10 +2556,19 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4">
@@ -2992,32 +2576,59 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change targets to goals
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data-template.xlsx
+++ b/tests/testthat/testdata/data-template.xlsx
@@ -831,13 +831,13 @@
     <t xml:space="preserve">Please enter information for your features into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input values to specify trade-offs for managing different biodiversity elements (e.g. species, habitat types) within your conservation planning exercise. To help prioritize implementation of specific management actions in specific sites, we require an estimate of the minimum amount of each feature you think is important to achieve across all of the sites (termed “target threshold amount”). For example, you could calculate these target threshold amounts as a percentage of the current amount of each feature (e.g. maybe you want to increase the amount of each feature by 50%)? Alternatively, these values could be guided using population viability analyses, statistical models, or expert elicitation. Please take care to ensure that each target value is in the same units as the expectation data. For example, the value in the cell B2 for this spreadsheet should be in the same unit as the values in the B column for all action expectation worksheets (i.e. worksheets starting with the word “Expectation”). To ensure that the prioritization process explicitly accounts for your objectives (i.e. what YOU think is important), you can also specify the relative importance (weight) of each feature. The default value is 1 such that all features are considered equally important. These values should be between 0 and 100. Greater values indicate greater importance. A weight of exactly 0 means that a feature is not important at all and does not “count” when comparing different conservation plans. Please note that these values can be changed later in the NCC Priority Actions App. After filling out this worksheet, every light gray cell should have a numerical value.</t>
+    <t xml:space="preserve">Specifically, we ask that you input values to specify trade-offs for managing different biodiversity elements (e.g. species, habitat types) within your conservation planning exercise. To help prioritize implementation of specific management actions in specific sites, we require percentage-based threshold values to specify the minimum amount of each feature you think is important to achieve across all of the sites (termed “goal”). Specifically, the goal values are expressed as a percentage of the maximum possible amount of each feature, assuming that the best possible action for each feature was implemented within each site (per the expecation data). To ensure that the prioritization process explicitly accounts for your objectives (i.e. what YOU think is important), you can also specify the relative importance (weight) of each feature. The default value is 1 such that all features are considered equally important. Greater values indicate greater importance. A weight of exactly 0 means that a feature is not important at all and does not “count” when comparing different conservation plans. Both goal and weight values should be between 0 and 100. Please note that these values can be changed later in the What To Do application. After filling out this worksheet, every light gray cell should have a numerical value.</t>
   </si>
   <si>
     <t xml:space="preserve">Feature ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Target threshold amount</t>
+    <t xml:space="preserve">Goal (%)</t>
   </si>
   <si>
     <t xml:space="preserve">Relative importance (weight)</t>
@@ -1233,7 +1233,7 @@
   <autoFilter ref="A3:C7"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Feature ID"/>
-    <tableColumn id="2" name="Target threshold amount"/>
+    <tableColumn id="2" name="Goal (%)"/>
     <tableColumn id="3" name="Relative importance (weight)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1905,7 +1905,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="20.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="33.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="18.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="38.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1987,7 +1987,7 @@
   <dataValidations count="2">
     <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="B4:B7">
       <formula1>0</formula1>
-      <formula2>1e+06</formula2>
+      <formula2>100</formula2>
     </dataValidation>
     <dataValidation type="decimal" operator="between" allowBlank="0" showInputMessage="1" showErrorMessage="1" sqref="C4:C7">
       <formula1>0</formula1>

</xml_diff>

<commit_message>
update test data to match config
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data-template.xlsx
+++ b/tests/testthat/testdata/data-template.xlsx
@@ -765,7 +765,7 @@
     <t xml:space="preserve">Please enter information for your sites into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input the longitude and latitude (in decimal degrees) of each site. If you have a shapefile with spatial locations (e.g. point localities, boundaries) of your sites, these can also be supplied in the NCC Priority Actions App. We also ask that you input the cost of implementing each management action (e.g. in Canadian Dollars) within each site. Please note that cost values should not be below zero (though they can equal zero) and not be greater than 1,000,000 (i.e. one million). As such, you might need to rescale your cost values. For example, if one of your cost values is “10000000” Canadian Dollars, instead of inputting values as Canadian Dollars, you could you input values as thousands of Canadian Dollars (i.e. “10000”). Please take care to ensure that all cost values are in the same units. After filling out this worksheet, every light gray cell should have a numerical value.</t>
+    <t xml:space="preserve">Specifically, we ask that you input the longitude and latitude (in decimal degrees) of each site. If you have a shapefile with spatial locations (e.g. point localities, boundaries) of your sites, these can also be supplied in the What To Do application. We also ask that you input the cost of implementing each management action (e.g. in Canadian Dollars) within each site. Please note that cost values should not be below zero (though they can equal zero) and not be greater than 1,000,000 (i.e. one million). As such, you might need to rescale your cost values. For example, if one of your cost values is “10000000” Canadian Dollars, instead of inputting values as Canadian Dollars, you could you input values as thousands of Canadian Dollars (i.e. “10000”). Please take care to ensure that all cost values are in the same units. After filling out this worksheet, every light gray cell should have a numerical value.</t>
   </si>
   <si>
     <t xml:space="preserve">Site ID</t>
@@ -810,7 +810,7 @@
     <t xml:space="preserve">Please enter feasibility information for your sites into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input data indicating which management actions are feasible to implement within each site. By default, all actions can be potentially implemented within each and every site. To specify that a certain a certain action cannot be implemented within a certain site, please enter value of “0”. You can also ensure that a certain site can ONLY have a certain action implemented within it, by specifying a value of “0” for every other action. This information, if you prefer, can also be specified within the NCC Priority Actions App---however, you will have to re-specify this information each and every time you open the NCC Priority Actions App.</t>
+    <t xml:space="preserve">Specifically, we ask that you input data indicating which management actions are feasible to implement within each site. By default, all actions can be potentially implemented within each and every site. To specify that a certain a certain action cannot be implemented within a certain site, please enter value of “0”. You can also ensure that a certain site can ONLY have a certain action implemented within it, by specifying a value of “0” for every other action. This information, if you prefer, can also be specified within the What To Do application---however, you will have to re-specify this information each and every time you open the application.</t>
   </si>
   <si>
     <t xml:space="preserve">Feasibility of “z”</t>

</xml_diff>

<commit_message>
update consequence sheet names per https://github.com/NCC-CNC/whattemplatemaker/issues/23
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data-template.xlsx
+++ b/tests/testthat/testdata/data-template.xlsx
@@ -9,11 +9,11 @@
     <sheet name="Site data" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Feasibility data" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Feature data" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Consequence of “z”" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Consequence of “x”" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Consequence of “c”" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Consequence of “v”" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Consequence of “b”" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="“z” consequence" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="“x” consequence" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="“c” consequence" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="“v” consequence" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="“b” consequence" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="metadata" sheetId="9" state="hidden" r:id="rId9"/>
   </sheets>
 </workbook>

</xml_diff>

<commit_message>
update template req for changes to whatdataio https://github.com/NCC-CNC/whattodo/issues/42 https://github.com/NCC-CNC/whattodo/issues/46 https://github.com/NCC-CNC/whattodo/issues/47
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data-template.xlsx
+++ b/tests/testthat/testdata/data-template.xlsx
@@ -831,7 +831,7 @@
     <t xml:space="preserve">Please enter information for your features into this worksheet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Specifically, we ask that you input values to specify trade-offs for managing different biodiversity elements (e.g. species, habitat types) within your conservation planning exercise. To help prioritize implementation of specific management actions in specific sites, we require percentage-based threshold values to specify the minimum amount of each feature you think is important to achieve across all of the sites (termed “goal”). Specifically, the goal values are expressed as a percentage of the maximum possible amount of each feature, assuming that the best possible action for each feature was implemented within each site (per the expecation data). To ensure that the prioritization process explicitly accounts for your objectives (i.e. what YOU think is important), you can also specify the relative importance (weight) of each feature. The default value is 1 such that all features are considered equally important. Greater values indicate greater importance. A weight of exactly 0 means that a feature is not important at all and does not “count” when comparing different conservation plans. Both goal and weight values should be between 0 and 100. Please note that these values can be changed later in the What To Do application. After filling out this worksheet, every light gray cell should have a numerical value.</t>
+    <t xml:space="preserve">Specifically, we ask that you input values to specify trade-offs for managing different biodiversity elements (e.g. species, habitat types) within your conservation planning exercise. To help prioritize implementation of specific management actions in specific sites, we require percentage-based threshold values to specify the minimum amount of each feature you think is important to achieve across all of the sites (termed “goal”). Specifically, the goal values are expressed as a percentage of the maximum possible amount of each feature, assuming that the best possible action for each feature was implemented within each site (per the expecation data). To ensure that the prioritization process explicitly accounts for your objectives (i.e. what YOU think is important), you can also specify the relative importance of each feature. The default value is 1 such that all features are considered equally important. Greater values indicate greater importance. An importance value of exactly 0 means that a feature is not important at all and does not “count” when comparing different conservation plans. Both goal and importance values should be between 0 and 100. Please note that these values can be changed later in the What To Do application. After filling out this worksheet, every light gray cell should have a numerical value.</t>
   </si>
   <si>
     <t xml:space="preserve">Feature ID</t>
@@ -840,7 +840,7 @@
     <t xml:space="preserve">Goal (%)</t>
   </si>
   <si>
-    <t xml:space="preserve">Relative importance (weight)</t>
+    <t xml:space="preserve">Relative importance</t>
   </si>
   <si>
     <t xml:space="preserve">a</t>
@@ -1234,7 +1234,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="Feature ID"/>
     <tableColumn id="2" name="Goal (%)"/>
-    <tableColumn id="3" name="Relative importance (weight)"/>
+    <tableColumn id="3" name="Relative importance"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1906,7 +1906,7 @@
   <cols>
     <col min="1" max="1" width="20.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="18.71" hidden="0" customWidth="1"/>
-    <col min="3" max="3" width="38.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="29.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">

</xml_diff>

<commit_message>
fix bug in current status of xlsx files
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data-template.xlsx
+++ b/tests/testthat/testdata/data-template.xlsx
@@ -1660,7 +1660,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -1679,7 +1679,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -1698,7 +1698,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -1735,9 +1735,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="0" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'meta'!$B$2:$B$6</xm:f>
+            <xm:f>'metadata'!$B$2:$B$6</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D6</xm:sqref>
         </x14:dataValidation>

</xml_diff>

<commit_message>
fix bug in template data
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/data-template.xlsx
+++ b/tests/testthat/testdata/data-template.xlsx
@@ -801,6 +801,9 @@
     <t xml:space="preserve"/>
   </si>
   <si>
+    <t xml:space="preserve">z</t>
+  </si>
+  <si>
     <t xml:space="preserve">w</t>
   </si>
   <si>
@@ -913,9 +916,6 @@
   </si>
   <si>
     <t xml:space="preserve">feature_descriptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">z</t>
   </si>
   <si>
     <t xml:space="preserve">Site q</t>
@@ -1660,7 +1660,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>12</v>
@@ -1679,7 +1679,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>12</v>
@@ -1698,7 +1698,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -1768,7 +1768,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1778,7 +1778,7 @@
     <row r="2" ht="100" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1790,19 +1790,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -1827,7 +1827,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>1</v>
@@ -1847,7 +1847,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>1</v>
@@ -1912,31 +1912,31 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" ht="250" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>12</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>12</v>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>12</v>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>12</v>
@@ -2023,7 +2023,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2032,7 +2032,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2043,16 +2043,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4">
@@ -2066,7 +2066,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2123,7 +2123,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2132,7 +2132,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2143,16 +2143,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4">
@@ -2166,7 +2166,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2223,7 +2223,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2232,7 +2232,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2243,16 +2243,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4">
@@ -2266,7 +2266,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2323,7 +2323,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2332,7 +2332,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2343,16 +2343,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4">
@@ -2366,7 +2366,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2375,7 +2375,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2423,7 +2423,7 @@
     <row r="1" ht="20" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2432,7 +2432,7 @@
     <row r="2" ht="160" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2443,16 +2443,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4">
@@ -2466,7 +2466,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2475,7 +2475,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2513,22 +2513,22 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2">
@@ -2536,10 +2536,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>52</v>
@@ -2553,13 +2553,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>56</v>
@@ -2573,13 +2573,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>60</v>
@@ -2599,7 +2599,7 @@
         <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>

</xml_diff>